<commit_message>
Can now set the first week of the excel sheet with employee information
</commit_message>
<xml_diff>
--- a/PayrollProgram/DIAZ, ELI - NEW FUNCTION CODE.xlsx
+++ b/PayrollProgram/DIAZ, ELI - NEW FUNCTION CODE.xlsx
@@ -1490,9 +1490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB165"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -1668,16 +1668,26 @@
       <c r="F5" s="110"/>
       <c r="G5" s="111"/>
       <c r="H5" s="28">
-        <v>3.5</v>
-      </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="49">
+        <v>2</v>
+      </c>
+      <c r="J5" s="49">
+        <v>3</v>
+      </c>
+      <c r="K5" s="49">
+        <v>4</v>
+      </c>
+      <c r="L5" s="49">
+        <v>5</v>
+      </c>
+      <c r="M5" s="49">
+        <v>6</v>
+      </c>
       <c r="N5" s="33">
         <f>SUM(H5:M5)</f>
-        <v>3.5</v>
+        <v>20</v>
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="11"/>
@@ -1704,16 +1714,26 @@
       <c r="F6" s="110"/>
       <c r="G6" s="111"/>
       <c r="H6" s="28">
-        <v>1</v>
-      </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="I6" s="49">
+        <v>2</v>
+      </c>
+      <c r="J6" s="49">
+        <v>3</v>
+      </c>
+      <c r="K6" s="49">
+        <v>4</v>
+      </c>
+      <c r="L6" s="49">
+        <v>5</v>
+      </c>
+      <c r="M6" s="49">
+        <v>6</v>
+      </c>
       <c r="N6" s="33">
         <f>SUM(H6:M6)</f>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O6" s="34"/>
       <c r="P6" s="11"/>
@@ -1740,16 +1760,26 @@
       <c r="F7" s="101"/>
       <c r="G7" s="123"/>
       <c r="H7" s="67">
+        <v>3</v>
+      </c>
+      <c r="I7" s="68">
         <v>2</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="J7" s="69">
+        <v>3</v>
+      </c>
+      <c r="K7" s="69">
+        <v>4</v>
+      </c>
+      <c r="L7" s="70">
+        <v>5</v>
+      </c>
+      <c r="M7" s="71">
+        <v>6</v>
+      </c>
       <c r="N7" s="72">
         <f t="shared" ref="N7:N13" si="0">SUM(H7:M7)</f>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="O7" s="35"/>
       <c r="P7" s="11"/>
@@ -1776,16 +1806,26 @@
       <c r="F8" s="101"/>
       <c r="G8" s="102"/>
       <c r="H8" s="61">
-        <v>8</v>
-      </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="61"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="62">
+        <v>0</v>
+      </c>
+      <c r="J8" s="63">
+        <v>0</v>
+      </c>
+      <c r="K8" s="63">
+        <v>0</v>
+      </c>
+      <c r="L8" s="64">
+        <v>0</v>
+      </c>
+      <c r="M8" s="61">
+        <v>0</v>
+      </c>
       <c r="N8" s="66">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O8" s="35"/>
       <c r="P8" s="11"/>
@@ -1812,16 +1852,26 @@
       <c r="F9" s="113"/>
       <c r="G9" s="114"/>
       <c r="H9" s="36">
-        <v>0.6</v>
-      </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="36"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="37">
+        <v>0</v>
+      </c>
+      <c r="J9" s="38">
+        <v>0</v>
+      </c>
+      <c r="K9" s="38">
+        <v>0</v>
+      </c>
+      <c r="L9" s="39">
+        <v>0</v>
+      </c>
+      <c r="M9" s="36">
+        <v>0</v>
+      </c>
       <c r="N9" s="33">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="O9" s="35"/>
       <c r="P9" s="11"/>
@@ -1848,16 +1898,26 @@
       <c r="F10" s="113"/>
       <c r="G10" s="114"/>
       <c r="H10" s="36">
-        <v>0.7</v>
-      </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="36"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="37">
+        <v>0</v>
+      </c>
+      <c r="J10" s="38">
+        <v>0</v>
+      </c>
+      <c r="K10" s="38">
+        <v>0</v>
+      </c>
+      <c r="L10" s="39">
+        <v>0</v>
+      </c>
+      <c r="M10" s="36">
+        <v>0</v>
+      </c>
       <c r="N10" s="33">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>6</v>
       </c>
       <c r="O10" s="35"/>
       <c r="P10" s="11"/>
@@ -1884,16 +1944,26 @@
       <c r="F11" s="101"/>
       <c r="G11" s="102"/>
       <c r="H11" s="36">
-        <v>1.2</v>
-      </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="94">
+        <v>0</v>
+      </c>
+      <c r="J11" s="38">
+        <v>0</v>
+      </c>
+      <c r="K11" s="38">
+        <v>0</v>
+      </c>
+      <c r="L11" s="39">
+        <v>0</v>
+      </c>
+      <c r="M11" s="36">
+        <v>0</v>
+      </c>
       <c r="N11" s="33">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>7</v>
       </c>
       <c r="O11" s="35"/>
       <c r="P11" s="11"/>
@@ -1920,16 +1990,26 @@
       <c r="F12" s="101"/>
       <c r="G12" s="102"/>
       <c r="H12" s="40">
-        <v>23</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="36"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="37">
+        <v>0</v>
+      </c>
+      <c r="J12" s="38">
+        <v>0</v>
+      </c>
+      <c r="K12" s="38">
+        <v>0</v>
+      </c>
+      <c r="L12" s="39">
+        <v>0</v>
+      </c>
+      <c r="M12" s="36">
+        <v>0</v>
+      </c>
       <c r="N12" s="33">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="O12" s="35"/>
       <c r="P12" s="11"/>
@@ -1956,16 +2036,26 @@
       <c r="F13" s="113"/>
       <c r="G13" s="114"/>
       <c r="H13" s="36">
-        <v>0</v>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="36"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="37">
+        <v>0</v>
+      </c>
+      <c r="J13" s="38">
+        <v>0</v>
+      </c>
+      <c r="K13" s="38">
+        <v>0</v>
+      </c>
+      <c r="L13" s="39">
+        <v>0</v>
+      </c>
+      <c r="M13" s="36">
+        <v>0</v>
+      </c>
       <c r="N13" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O13" s="35"/>
       <c r="P13" s="11"/>
@@ -1993,31 +2083,31 @@
       <c r="G14" s="108"/>
       <c r="H14" s="24">
         <f t="shared" ref="H14:N14" si="1">SUM(H5:H13)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I14" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J14" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K14" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L14" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M14" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N14" s="24">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="O14" s="52"/>
       <c r="P14" s="53" t="s">
@@ -2109,7 +2199,7 @@
       <c r="O16" s="50"/>
       <c r="P16" s="73">
         <f t="shared" ref="P16:P25" si="2">SUM(N5,N16)</f>
-        <v>3.5</v>
+        <v>20</v>
       </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -2146,7 +2236,7 @@
       <c r="O17" s="50"/>
       <c r="P17" s="73">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -2183,7 +2273,7 @@
       <c r="O18" s="50"/>
       <c r="P18" s="73">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
@@ -2220,7 +2310,7 @@
       <c r="O19" s="50"/>
       <c r="P19" s="74">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -2257,7 +2347,7 @@
       <c r="O20" s="50"/>
       <c r="P20" s="60">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -2294,7 +2384,7 @@
       <c r="O21" s="50"/>
       <c r="P21" s="60">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>6</v>
       </c>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
@@ -2331,7 +2421,7 @@
       <c r="O22" s="50"/>
       <c r="P22" s="60">
         <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>7</v>
       </c>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
@@ -2368,7 +2458,7 @@
       <c r="O23" s="50"/>
       <c r="P23" s="60">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
@@ -2405,7 +2495,7 @@
       <c r="O24" s="50"/>
       <c r="P24" s="60">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
@@ -2460,7 +2550,7 @@
       <c r="O25" s="51"/>
       <c r="P25" s="60">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>

</xml_diff>

<commit_message>
Now writes hours of both sections of excel file.
</commit_message>
<xml_diff>
--- a/PayrollProgram/DIAZ, ELI - NEW FUNCTION CODE.xlsx
+++ b/PayrollProgram/DIAZ, ELI - NEW FUNCTION CODE.xlsx
@@ -974,6 +974,80 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -986,15 +1060,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1013,73 +1078,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1492,7 +1492,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -1518,44 +1518,44 @@
       <c r="B1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
       <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="122" t="s">
+      <c r="I1" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="122"/>
+      <c r="J1" s="98"/>
       <c r="K1" s="46">
         <v>14</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="116">
+      <c r="M1" s="112">
         <v>42734</v>
       </c>
-      <c r="N1" s="117"/>
+      <c r="N1" s="113"/>
     </row>
     <row r="2" spans="2:28" s="18" customFormat="1" ht="24" customHeight="1">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="125" t="s">
+      <c r="C2" s="114"/>
+      <c r="D2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
       <c r="H2" s="17"/>
       <c r="I2" s="76"/>
       <c r="J2" s="77"/>
@@ -1565,14 +1565,14 @@
       <c r="N2" s="19"/>
     </row>
     <row r="3" spans="2:28" s="44" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="129"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="111"/>
       <c r="H3" s="79">
         <f>M1-13</f>
         <v>42721</v>
@@ -1659,35 +1659,35 @@
       <c r="AB4" s="15"/>
     </row>
     <row r="5" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="111"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="28">
         <v>0</v>
       </c>
       <c r="I5" s="49">
+        <v>1</v>
+      </c>
+      <c r="J5" s="49">
         <v>2</v>
       </c>
-      <c r="J5" s="49">
+      <c r="K5" s="49">
         <v>3</v>
       </c>
-      <c r="K5" s="49">
+      <c r="L5" s="49">
         <v>4</v>
       </c>
-      <c r="L5" s="49">
+      <c r="M5" s="49">
         <v>5</v>
-      </c>
-      <c r="M5" s="49">
-        <v>6</v>
       </c>
       <c r="N5" s="33">
         <f>SUM(H5:M5)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="11"/>
@@ -1705,35 +1705,35 @@
       <c r="AB5" s="11"/>
     </row>
     <row r="6" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="111"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
       <c r="H6" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K6" s="49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L6" s="49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M6" s="49">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N6" s="33">
         <f>SUM(H6:M6)</f>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="O6" s="34"/>
       <c r="P6" s="11"/>
@@ -1751,35 +1751,35 @@
       <c r="AB6" s="11"/>
     </row>
     <row r="7" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="123"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="102"/>
       <c r="H7" s="67">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="69">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L7" s="70">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M7" s="71">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N7" s="72">
         <f t="shared" ref="N7:N13" si="0">SUM(H7:M7)</f>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="O7" s="35"/>
       <c r="P7" s="11"/>
@@ -1797,16 +1797,16 @@
       <c r="AB7" s="11"/>
     </row>
     <row r="8" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="102"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97"/>
       <c r="H8" s="61">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8" s="62">
         <v>0</v>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="N8" s="66">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O8" s="35"/>
       <c r="P8" s="11"/>
@@ -1843,16 +1843,16 @@
       <c r="AB8" s="11"/>
     </row>
     <row r="9" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="114"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="105"/>
       <c r="H9" s="36">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I9" s="37">
         <v>0</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="N9" s="33">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O9" s="35"/>
       <c r="P9" s="11"/>
@@ -1889,16 +1889,16 @@
       <c r="AB9" s="11"/>
     </row>
     <row r="10" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="114"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="105"/>
       <c r="H10" s="36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I10" s="37">
         <v>0</v>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="N10" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O10" s="35"/>
       <c r="P10" s="11"/>
@@ -1935,16 +1935,16 @@
       <c r="AB10" s="11"/>
     </row>
     <row r="11" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B11" s="100" t="s">
+      <c r="B11" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="97"/>
       <c r="H11" s="36">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I11" s="94">
         <v>0</v>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="N11" s="33">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O11" s="35"/>
       <c r="P11" s="11"/>
@@ -1981,16 +1981,16 @@
       <c r="AB11" s="11"/>
     </row>
     <row r="12" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="97"/>
       <c r="H12" s="40">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I12" s="37">
         <v>0</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="N12" s="33">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O12" s="35"/>
       <c r="P12" s="11"/>
@@ -2027,35 +2027,35 @@
       <c r="AB12" s="11"/>
     </row>
     <row r="13" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="114"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="105"/>
       <c r="H13" s="36">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I13" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L13" s="39">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M13" s="36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N13" s="33">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="O13" s="35"/>
       <c r="P13" s="11"/>
@@ -2073,41 +2073,41 @@
       <c r="AB13" s="11"/>
     </row>
     <row r="14" spans="2:28" s="55" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B14" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="108"/>
+      <c r="B14" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="128"/>
       <c r="H14" s="24">
         <f t="shared" ref="H14:N14" si="1">SUM(H5:H13)</f>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I14" s="24">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J14" s="24">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K14" s="24">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L14" s="24">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M14" s="24">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="N14" s="24">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="O14" s="52"/>
       <c r="P14" s="53" t="s">
@@ -2127,12 +2127,12 @@
       <c r="AB14" s="54"/>
     </row>
     <row r="15" spans="2:28" s="58" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B15" s="119"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="121"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="117"/>
       <c r="H15" s="90">
         <f>+M3+1</f>
         <v>42728</v>
@@ -2178,28 +2178,40 @@
       <c r="AB15" s="57"/>
     </row>
     <row r="16" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="32">
+        <v>6</v>
+      </c>
+      <c r="I16" s="49">
+        <v>7</v>
+      </c>
+      <c r="J16" s="49">
+        <v>8</v>
+      </c>
+      <c r="K16" s="49">
+        <v>9</v>
+      </c>
+      <c r="L16" s="49">
+        <v>10</v>
+      </c>
+      <c r="M16" s="49">
+        <v>12</v>
+      </c>
       <c r="N16" s="33">
         <f>SUM(H16:M16)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="O16" s="50"/>
       <c r="P16" s="73">
         <f t="shared" ref="P16:P25" si="2">SUM(N5,N16)</f>
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -2215,20 +2227,32 @@
       <c r="AB16" s="11"/>
     </row>
     <row r="17" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="110"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="71"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="71">
+        <v>0</v>
+      </c>
+      <c r="I17" s="68">
+        <v>0</v>
+      </c>
+      <c r="J17" s="69">
+        <v>0</v>
+      </c>
+      <c r="K17" s="69">
+        <v>0</v>
+      </c>
+      <c r="L17" s="70">
+        <v>0</v>
+      </c>
+      <c r="M17" s="71">
+        <v>0</v>
+      </c>
       <c r="N17" s="72">
         <f>SUM(H17:M17)</f>
         <v>0</v>
@@ -2236,7 +2260,7 @@
       <c r="O17" s="50"/>
       <c r="P17" s="73">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -2252,20 +2276,32 @@
       <c r="AB17" s="11"/>
     </row>
     <row r="18" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B18" s="100" t="s">
+      <c r="B18" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="71"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="71">
+        <v>0</v>
+      </c>
+      <c r="I18" s="68">
+        <v>0</v>
+      </c>
+      <c r="J18" s="69">
+        <v>0</v>
+      </c>
+      <c r="K18" s="69">
+        <v>0</v>
+      </c>
+      <c r="L18" s="70">
+        <v>0</v>
+      </c>
+      <c r="M18" s="71">
+        <v>0</v>
+      </c>
       <c r="N18" s="72">
         <f>SUM(H18:M18)</f>
         <v>0</v>
@@ -2273,7 +2309,7 @@
       <c r="O18" s="50"/>
       <c r="P18" s="73">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
@@ -2289,20 +2325,32 @@
       <c r="AB18" s="11"/>
     </row>
     <row r="19" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="65"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="61">
+        <v>0</v>
+      </c>
+      <c r="I19" s="62">
+        <v>0</v>
+      </c>
+      <c r="J19" s="63">
+        <v>0</v>
+      </c>
+      <c r="K19" s="63">
+        <v>0</v>
+      </c>
+      <c r="L19" s="64">
+        <v>0</v>
+      </c>
+      <c r="M19" s="65">
+        <v>0</v>
+      </c>
       <c r="N19" s="66">
         <f>SUM(H19:M19)</f>
         <v>0</v>
@@ -2310,7 +2358,7 @@
       <c r="O19" s="50"/>
       <c r="P19" s="74">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -2326,20 +2374,32 @@
       <c r="AB19" s="11"/>
     </row>
     <row r="20" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B20" s="112" t="s">
+      <c r="B20" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="36"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="36">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37">
+        <v>0</v>
+      </c>
+      <c r="J20" s="38">
+        <v>0</v>
+      </c>
+      <c r="K20" s="38">
+        <v>0</v>
+      </c>
+      <c r="L20" s="39">
+        <v>0</v>
+      </c>
+      <c r="M20" s="36">
+        <v>0</v>
+      </c>
       <c r="N20" s="33">
         <f t="shared" ref="N20:N24" si="3">SUM(H20:M20)</f>
         <v>0</v>
@@ -2347,7 +2407,7 @@
       <c r="O20" s="50"/>
       <c r="P20" s="60">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -2363,20 +2423,32 @@
       <c r="AB20" s="11"/>
     </row>
     <row r="21" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="114"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="36">
+        <v>0</v>
+      </c>
+      <c r="I21" s="37">
+        <v>0</v>
+      </c>
+      <c r="J21" s="38">
+        <v>0</v>
+      </c>
+      <c r="K21" s="38">
+        <v>0</v>
+      </c>
+      <c r="L21" s="38">
+        <v>0</v>
+      </c>
+      <c r="M21" s="38">
+        <v>0</v>
+      </c>
       <c r="N21" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2384,7 +2456,7 @@
       <c r="O21" s="50"/>
       <c r="P21" s="60">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
@@ -2400,20 +2472,32 @@
       <c r="AB21" s="11"/>
     </row>
     <row r="22" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="41"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="36">
+        <v>0</v>
+      </c>
+      <c r="I22" s="37">
+        <v>0</v>
+      </c>
+      <c r="J22" s="38">
+        <v>0</v>
+      </c>
+      <c r="K22" s="38">
+        <v>0</v>
+      </c>
+      <c r="L22" s="39">
+        <v>0</v>
+      </c>
+      <c r="M22" s="41">
+        <v>0</v>
+      </c>
       <c r="N22" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2421,7 +2505,7 @@
       <c r="O22" s="50"/>
       <c r="P22" s="60">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
@@ -2437,20 +2521,32 @@
       <c r="AB22" s="11"/>
     </row>
     <row r="23" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="32"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="40">
+        <v>0</v>
+      </c>
+      <c r="I23" s="29">
+        <v>0</v>
+      </c>
+      <c r="J23" s="30">
+        <v>0</v>
+      </c>
+      <c r="K23" s="30">
+        <v>0</v>
+      </c>
+      <c r="L23" s="31">
+        <v>0</v>
+      </c>
+      <c r="M23" s="32">
+        <v>0</v>
+      </c>
       <c r="N23" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -2458,7 +2554,7 @@
       <c r="O23" s="50"/>
       <c r="P23" s="60">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
@@ -2474,28 +2570,40 @@
       <c r="AB23" s="11"/>
     </row>
     <row r="24" spans="2:28" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="32"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="32">
+        <v>6</v>
+      </c>
+      <c r="I24" s="29">
+        <v>7</v>
+      </c>
+      <c r="J24" s="30">
+        <v>8</v>
+      </c>
+      <c r="K24" s="30">
+        <v>9</v>
+      </c>
+      <c r="L24" s="31">
+        <v>10</v>
+      </c>
+      <c r="M24" s="32">
+        <v>11</v>
+      </c>
       <c r="N24" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="O24" s="50"/>
       <c r="P24" s="60">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
@@ -2511,46 +2619,46 @@
       <c r="AB24" s="11"/>
     </row>
     <row r="25" spans="2:28" s="14" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B25" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="107"/>
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="108"/>
+      <c r="B25" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="127"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="128"/>
       <c r="H25" s="24">
         <f t="shared" ref="H25:M25" si="4">SUM(H16:H24)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I25" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J25" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K25" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L25" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M25" s="24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N25" s="24">
         <f t="shared" ref="N25" si="5">SUM(N16:N24)</f>
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="O25" s="51"/>
       <c r="P25" s="60">
         <f t="shared" si="2"/>
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
@@ -2566,23 +2674,23 @@
       <c r="AB25" s="13"/>
     </row>
     <row r="26" spans="2:28" ht="36.75" customHeight="1">
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="105"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="120"/>
+      <c r="G26" s="120"/>
+      <c r="H26" s="120"/>
       <c r="I26" s="20"/>
       <c r="J26" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="98"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="99"/>
-      <c r="N26" s="99"/>
+      <c r="K26" s="121"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
       <c r="O26" s="4"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
@@ -2608,12 +2716,12 @@
       <c r="H27" s="10"/>
       <c r="I27" s="8"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="115" t="s">
+      <c r="K27" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
-      <c r="N27" s="115"/>
+      <c r="L27" s="129"/>
+      <c r="M27" s="129"/>
+      <c r="N27" s="129"/>
       <c r="O27" s="4"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -2630,25 +2738,25 @@
       <c r="AB27" s="6"/>
     </row>
     <row r="28" spans="2:28" ht="33.75" customHeight="1">
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="96" t="s">
+      <c r="C28" s="124"/>
+      <c r="D28" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="119"/>
       <c r="I28" s="4"/>
       <c r="J28" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="95"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="118"/>
+      <c r="M28" s="118"/>
+      <c r="N28" s="118"/>
       <c r="O28" s="4"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -3155,24 +3263,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B17:G17"/>
     <mergeCell ref="K28:N28"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D26:H26"/>
@@ -3189,6 +3279,24 @@
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="K27:N27"/>
     <mergeCell ref="B22:G22"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.1" footer="0"/>

</xml_diff>